<commit_message>
Modified HKD and JPY 05.11.2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="555" windowWidth="29040" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="435" yWindow="555" windowWidth="19440" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
   <si>
     <t>Earliest Date</t>
   </si>
@@ -523,6 +523,9 @@
   <si>
     <t>Instruments
 Selected</t>
+  </si>
+  <si>
+    <t>Settl Days</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1792,7 @@
     <row r="1" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="77" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Oct 13 2014 15:51:57</v>
+        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May  5 2015 15:27:06</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1988,7 +1991,7 @@
       </c>
       <c r="D14" s="102" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>HKDYCSTD#0001</v>
+        <v>HKDYCSTD#0008</v>
       </c>
       <c r="E14" s="80"/>
       <c r="F14" s="122"/>
@@ -2114,7 +2117,7 @@
       <c r="B23" s="78"/>
       <c r="C23" s="113">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="D23" s="114">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
@@ -2127,11 +2130,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="115">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>49251</v>
+        <v>49443</v>
       </c>
       <c r="D24" s="90">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>0.57776018256954154</v>
+        <v>0.61733372763186234</v>
       </c>
       <c r="E24" s="80"/>
       <c r="F24" s="122"/>
@@ -2260,7 +2263,7 @@
     <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>Deposits!E3</f>
-        <v>obj_00136#0001</v>
+        <v>obj_00121#0002</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A2)</f>
@@ -2268,7 +2271,7 @@
       </c>
       <c r="C2" s="5">
         <f>_xll.qlRateHelperQuoteValue($A2,Trigger)</f>
-        <v>4.9790000000000001E-4</v>
+        <v>4.7990000000000006E-4</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="b">
@@ -2282,17 +2285,17 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I2" s="12">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>Deposits!E4</f>
-        <v>obj_0013a#0001</v>
+        <v>obj_00127#0002</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A3)</f>
@@ -2300,7 +2303,7 @@
       </c>
       <c r="C3" s="5">
         <f>_xll.qlRateHelperQuoteValue($A3,Trigger)</f>
-        <v>1.1357000000000001E-3</v>
+        <v>9.9140000000000014E-4</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="b">
@@ -2314,17 +2317,17 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I3" s="12">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
-        <v>41950</v>
+        <v>42142</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
         <f>Deposits!E5</f>
-        <v>obj_00139#0001</v>
+        <v>obj_00126#0002</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A4)</f>
@@ -2332,7 +2335,7 @@
       </c>
       <c r="C4" s="5">
         <f>_xll.qlRateHelperQuoteValue($A4,Trigger)</f>
-        <v>1.5713999999999999E-3</v>
+        <v>1.3820000000000002E-3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="b">
@@ -2346,17 +2349,17 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I4" s="12">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>41957</v>
+        <v>42150</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f>Deposits!E6</f>
-        <v>obj_0013c#0001</v>
+        <v>obj_00129#0002</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A5)</f>
@@ -2364,7 +2367,7 @@
       </c>
       <c r="C5" s="5">
         <f>_xll.qlRateHelperQuoteValue($A5,Trigger)</f>
-        <v>2.3070999999999999E-3</v>
+        <v>2.4043000000000003E-3</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="b">
@@ -2378,17 +2381,17 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I5" s="12">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
-        <v>41971</v>
+        <v>42166</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>Deposits!E7</f>
-        <v>obj_00138#0001</v>
+        <v>obj_00125#0002</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A6)</f>
@@ -2396,7 +2399,7 @@
       </c>
       <c r="C6" s="5">
         <f>_xll.qlRateHelperQuoteValue($A6,Trigger)</f>
-        <v>3.1713999999999996E-3</v>
+        <v>3.0371000000000005E-3</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="b">
@@ -2410,17 +2413,17 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($A6,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I6" s="12">
         <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
-        <v>42004</v>
+        <v>42198</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f>Deposits!E8</f>
-        <v>obj_0013d#0001</v>
+        <v>obj_00122#0002</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A7)</f>
@@ -2428,7 +2431,7 @@
       </c>
       <c r="C7" s="5">
         <f>_xll.qlRateHelperQuoteValue($A7,Trigger)</f>
-        <v>3.7713999999999998E-3</v>
+        <v>3.8600000000000001E-3</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="b">
@@ -2442,17 +2445,17 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I7" s="12">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>42034</v>
+        <v>42227</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="str">
         <f>Deposits!E9</f>
-        <v>obj_0013b#0001</v>
+        <v>obj_00128#0002</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A8)</f>
@@ -2460,7 +2463,7 @@
       </c>
       <c r="C8" s="5">
         <f>_xll.qlRateHelperQuoteValue($A8,Trigger)</f>
-        <v>5.3785999999999999E-3</v>
+        <v>5.4136000000000011E-3</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="b">
@@ -2474,17 +2477,17 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I8" s="12">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>42124</v>
+        <v>42319</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>Deposits!E10</f>
-        <v>obj_0013e#0001</v>
+        <v>obj_00124#0002</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A9)</f>
@@ -2506,17 +2509,17 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($A9,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I9" s="12">
         <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
-        <v>42216</v>
+        <v>42411</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>Deposits!E11</f>
-        <v>obj_00137#0001</v>
+        <v>obj_00123#0002</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(A10)</f>
@@ -2524,7 +2527,7 @@
       </c>
       <c r="C10" s="8">
         <f>_xll.qlRateHelperQuoteValue($A10,Trigger)</f>
-        <v>8.3929E-3</v>
+        <v>8.4153000000000006E-3</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="b">
@@ -2538,17 +2541,17 @@
       </c>
       <c r="H10" s="13">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I10" s="14">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>42307</v>
+        <v>42501</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
-        <f>Swaps!K6</f>
-        <v>obj_0011f#0001</v>
+        <f>Swaps!L6</f>
+        <v>obj_00157#0003</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A11)</f>
@@ -2556,7 +2559,7 @@
       </c>
       <c r="C11" s="5">
         <f>_xll.qlRateHelperQuoteValue($A11,Trigger)</f>
-        <v>4.3E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="D11" s="5">
         <f>_xll.qlSwapRateHelperSpread($A11,Trigger)</f>
@@ -2574,17 +2577,17 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($A11,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I11" s="12">
         <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
-        <v>42311</v>
+        <v>42502</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
-        <f>Swaps!K7</f>
-        <v>obj_00132#0001</v>
+        <f>Swaps!L7</f>
+        <v>obj_00169#0003</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A12)</f>
@@ -2610,17 +2613,17 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I12" s="12">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>42403</v>
+        <v>42594</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
-        <f>Swaps!K8</f>
-        <v>obj_00125#0001</v>
+        <f>Swaps!L8</f>
+        <v>obj_00166#0003</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A13)</f>
@@ -2628,7 +2631,7 @@
       </c>
       <c r="C13" s="5">
         <f>_xll.qlRateHelperQuoteValue($A13,Trigger)</f>
-        <v>5.7000000000000002E-3</v>
+        <v>6.5000000000000006E-3</v>
       </c>
       <c r="D13" s="5">
         <f>_xll.qlSwapRateHelperSpread($A13,Trigger)</f>
@@ -2646,17 +2649,17 @@
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I13" s="12">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
-        <v>42493</v>
+        <v>42688</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="str">
-        <f>Swaps!K9</f>
-        <v>obj_00123#0001</v>
+        <f>Swaps!L9</f>
+        <v>obj_00163#0003</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A14)</f>
@@ -2682,17 +2685,17 @@
       </c>
       <c r="H14" s="11">
         <f>_xll.qlRateHelperEarliestDate($A14,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I14" s="12">
         <f>_xll.qlRateHelperLatestDate($A14,Trigger)</f>
-        <v>42585</v>
+        <v>42779</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
-        <f>Swaps!K10</f>
-        <v>obj_00130#0001</v>
+        <f>Swaps!L10</f>
+        <v>obj_00160#0003</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A15)</f>
@@ -2700,7 +2703,7 @@
       </c>
       <c r="C15" s="5">
         <f>_xll.qlRateHelperQuoteValue($A15,Trigger)</f>
-        <v>7.4999999999999997E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="D15" s="5">
         <f>_xll.qlSwapRateHelperSpread($A15,Trigger)</f>
@@ -2718,17 +2721,17 @@
       </c>
       <c r="H15" s="11">
         <f>_xll.qlRateHelperEarliestDate($A15,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I15" s="12">
         <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
-        <v>42677</v>
+        <v>42867</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
-        <f>Swaps!K11</f>
-        <v>obj_0012d#0001</v>
+        <f>Swaps!L11</f>
+        <v>obj_0015d#0003</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A16)</f>
@@ -2736,7 +2739,7 @@
       </c>
       <c r="C16" s="5">
         <f>_xll.qlRateHelperQuoteValue($A16,Trigger)</f>
-        <v>1.1299999999999999E-2</v>
+        <v>1.14E-2</v>
       </c>
       <c r="D16" s="5">
         <f>_xll.qlSwapRateHelperSpread($A16,Trigger)</f>
@@ -2754,17 +2757,17 @@
       </c>
       <c r="H16" s="11">
         <f>_xll.qlRateHelperEarliestDate($A16,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I16" s="12">
         <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
-        <v>43042</v>
+        <v>43234</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
-        <f>Swaps!K12</f>
-        <v>obj_00126#0001</v>
+        <f>Swaps!L12</f>
+        <v>obj_0015a#0003</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A17)</f>
@@ -2772,7 +2775,7 @@
       </c>
       <c r="C17" s="5">
         <f>_xll.qlRateHelperQuoteValue($A17,Trigger)</f>
-        <v>1.4499999999999999E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="D17" s="5">
         <f>_xll.qlSwapRateHelperSpread($A17,Trigger)</f>
@@ -2790,17 +2793,17 @@
       </c>
       <c r="H17" s="11">
         <f>_xll.qlRateHelperEarliestDate($A17,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I17" s="12">
         <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
-        <v>43409</v>
+        <v>43598</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
-        <f>Swaps!K13</f>
-        <v>obj_00121#0001</v>
+        <f>Swaps!L13</f>
+        <v>obj_0016c#0003</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A18)</f>
@@ -2808,7 +2811,7 @@
       </c>
       <c r="C18" s="5">
         <f>_xll.qlRateHelperQuoteValue($A18,Trigger)</f>
-        <v>1.7000000000000001E-2</v>
+        <v>1.5600000000000001E-2</v>
       </c>
       <c r="D18" s="5">
         <f>_xll.qlSwapRateHelperSpread($A18,Trigger)</f>
@@ -2826,17 +2829,17 @@
       </c>
       <c r="H18" s="11">
         <f>_xll.qlRateHelperEarliestDate($A18,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I18" s="12">
         <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
-        <v>43773</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
-        <f>Swaps!K14</f>
-        <v>obj_0012f#0001</v>
+        <f>Swaps!L14</f>
+        <v>obj_0016a#0003</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A19)</f>
@@ -2862,17 +2865,17 @@
       </c>
       <c r="H19" s="11">
         <f>_xll.qlRateHelperEarliestDate($A19,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I19" s="12">
         <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
-        <v>44138</v>
+        <v>44328</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="str">
-        <f>Swaps!K15</f>
-        <v>obj_00122#0001</v>
+        <f>Swaps!L15</f>
+        <v>obj_00168#0003</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A20)</f>
@@ -2880,7 +2883,7 @@
       </c>
       <c r="C20" s="5">
         <f>_xll.qlRateHelperQuoteValue($A20,Trigger)</f>
-        <v>2.0199999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="D20" s="5">
         <f>_xll.qlSwapRateHelperSpread($A20,Trigger)</f>
@@ -2898,17 +2901,17 @@
       </c>
       <c r="H20" s="11">
         <f>_xll.qlRateHelperEarliestDate($A20,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I20" s="12">
         <f>_xll.qlRateHelperLatestDate($A20,Trigger)</f>
-        <v>44503</v>
+        <v>44693</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
-        <f>Swaps!K16</f>
-        <v>obj_00129#0001</v>
+        <f>Swaps!L16</f>
+        <v>obj_00165#0003</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A21)</f>
@@ -2934,17 +2937,17 @@
       </c>
       <c r="H21" s="11">
         <f>_xll.qlRateHelperEarliestDate($A21,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I21" s="12">
         <f>_xll.qlRateHelperLatestDate($A21,Trigger)</f>
-        <v>44868</v>
+        <v>45058</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
-        <f>Swaps!K17</f>
-        <v>obj_0012b#0001</v>
+        <f>Swaps!L17</f>
+        <v>obj_00162#0003</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A22)</f>
@@ -2970,17 +2973,17 @@
       </c>
       <c r="H22" s="11">
         <f>_xll.qlRateHelperEarliestDate($A22,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I22" s="12">
         <f>_xll.qlRateHelperLatestDate($A22,Trigger)</f>
-        <v>45233</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="str">
-        <f>Swaps!K18</f>
-        <v>obj_00120#0001</v>
+        <f>Swaps!L18</f>
+        <v>obj_0015f#0003</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A23)</f>
@@ -2988,7 +2991,7 @@
       </c>
       <c r="C23" s="5">
         <f>_xll.qlRateHelperQuoteValue($A23,Trigger)</f>
-        <v>2.3E-2</v>
+        <v>2.06E-2</v>
       </c>
       <c r="D23" s="5">
         <f>_xll.qlSwapRateHelperSpread($A23,Trigger)</f>
@@ -3006,17 +3009,17 @@
       </c>
       <c r="H23" s="11">
         <f>_xll.qlRateHelperEarliestDate($A23,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I23" s="12">
         <f>_xll.qlRateHelperLatestDate($A23,Trigger)</f>
-        <v>45600</v>
+        <v>45789</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
-        <f>Swaps!K19</f>
-        <v>obj_00124#0001</v>
+        <f>Swaps!L19</f>
+        <v>obj_0015c#0003</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A24)</f>
@@ -3042,17 +3045,17 @@
       </c>
       <c r="H24" s="11">
         <f>_xll.qlRateHelperEarliestDate($A24,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I24" s="12">
         <f>_xll.qlRateHelperLatestDate($A24,Trigger)</f>
-        <v>45964</v>
+        <v>46154</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
-        <f>Swaps!K20</f>
-        <v>obj_00134#0001</v>
+        <f>Swaps!L20</f>
+        <v>obj_00159#0003</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A25)</f>
@@ -3060,7 +3063,7 @@
       </c>
       <c r="C25" s="5">
         <f>_xll.qlRateHelperQuoteValue($A25,Trigger)</f>
-        <v>2.4199999999999999E-2</v>
+        <v>2.1399999999999995E-2</v>
       </c>
       <c r="D25" s="5">
         <f>_xll.qlSwapRateHelperSpread($A25,Trigger)</f>
@@ -3078,17 +3081,17 @@
       </c>
       <c r="H25" s="11">
         <f>_xll.qlRateHelperEarliestDate($A25,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I25" s="12">
         <f>_xll.qlRateHelperLatestDate($A25,Trigger)</f>
-        <v>46329</v>
+        <v>46519</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="str">
-        <f>Swaps!K21</f>
-        <v>obj_0012e#0001</v>
+        <f>Swaps!L21</f>
+        <v>obj_0016b#0003</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A26)</f>
@@ -3114,17 +3117,17 @@
       </c>
       <c r="H26" s="11">
         <f>_xll.qlRateHelperEarliestDate($A26,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I26" s="12">
         <f>_xll.qlRateHelperLatestDate($A26,Trigger)</f>
-        <v>46694</v>
+        <v>46885</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="str">
-        <f>Swaps!K22</f>
-        <v>obj_0012c#0001</v>
+        <f>Swaps!L22</f>
+        <v>obj_0016d#0003</v>
       </c>
       <c r="B27" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A27)</f>
@@ -3150,17 +3153,17 @@
       </c>
       <c r="H27" s="11">
         <f>_xll.qlRateHelperEarliestDate($A27,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I27" s="12">
         <f>_xll.qlRateHelperLatestDate($A27,Trigger)</f>
-        <v>47060</v>
+        <v>47252</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
-        <f>Swaps!K23</f>
-        <v>obj_00133#0001</v>
+        <f>Swaps!L23</f>
+        <v>obj_00167#0003</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A28)</f>
@@ -3168,7 +3171,7 @@
       </c>
       <c r="C28" s="5">
         <f>_xll.qlRateHelperQuoteValue($A28,Trigger)</f>
-        <v>2.5300000000000003E-2</v>
+        <v>2.2199999999999998E-2</v>
       </c>
       <c r="D28" s="5">
         <f>_xll.qlSwapRateHelperSpread($A28,Trigger)</f>
@@ -3186,17 +3189,17 @@
       </c>
       <c r="H28" s="11">
         <f>_xll.qlRateHelperEarliestDate($A28,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I28" s="12">
         <f>_xll.qlRateHelperLatestDate($A28,Trigger)</f>
-        <v>47427</v>
+        <v>47616</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="str">
-        <f>Swaps!K24</f>
-        <v>obj_00135#0001</v>
+        <f>Swaps!L24</f>
+        <v>obj_00164#0003</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A29)</f>
@@ -3222,17 +3225,17 @@
       </c>
       <c r="H29" s="11">
         <f>_xll.qlRateHelperEarliestDate($A29,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I29" s="12">
         <f>_xll.qlRateHelperLatestDate($A29,Trigger)</f>
-        <v>47791</v>
+        <v>47980</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="str">
-        <f>Swaps!K25</f>
-        <v>obj_00131#0001</v>
+        <f>Swaps!L25</f>
+        <v>obj_00161#0003</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A30)</f>
@@ -3258,17 +3261,17 @@
       </c>
       <c r="H30" s="11">
         <f>_xll.qlRateHelperEarliestDate($A30,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I30" s="12">
         <f>_xll.qlRateHelperLatestDate($A30,Trigger)</f>
-        <v>48155</v>
+        <v>48346</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="str">
-        <f>Swaps!K26</f>
-        <v>obj_00127#0001</v>
+        <f>Swaps!L26</f>
+        <v>obj_0015e#0003</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A31)</f>
@@ -3294,17 +3297,17 @@
       </c>
       <c r="H31" s="11">
         <f>_xll.qlRateHelperEarliestDate($A31,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I31" s="12">
         <f>_xll.qlRateHelperLatestDate($A31,Trigger)</f>
-        <v>48521</v>
+        <v>48711</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="str">
-        <f>Swaps!K27</f>
-        <v>obj_0012a#0001</v>
+        <f>Swaps!L27</f>
+        <v>obj_0015b#0003</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A32)</f>
@@ -3330,17 +3333,17 @@
       </c>
       <c r="H32" s="11">
         <f>_xll.qlRateHelperEarliestDate($A32,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I32" s="12">
         <f>_xll.qlRateHelperLatestDate($A32,Trigger)</f>
-        <v>48886</v>
+        <v>49076</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
-        <f>Swaps!K28</f>
-        <v>obj_00128#0001</v>
+        <f>Swaps!L28</f>
+        <v>obj_00158#0003</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A33)</f>
@@ -3348,7 +3351,7 @@
       </c>
       <c r="C33" s="5">
         <f>_xll.qlRateHelperQuoteValue($A33,Trigger)</f>
-        <v>2.6600000000000002E-2</v>
+        <v>2.35E-2</v>
       </c>
       <c r="D33" s="5">
         <f>_xll.qlSwapRateHelperSpread($A33,Trigger)</f>
@@ -3366,11 +3369,11 @@
       </c>
       <c r="H33" s="11">
         <f>_xll.qlRateHelperEarliestDate($A33,Trigger)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I33" s="12">
         <f>_xll.qlRateHelperLatestDate($A33,Trigger)</f>
-        <v>49251</v>
+        <v>49443</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3451,7 +3454,7 @@
       </c>
       <c r="D2" s="21" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_0013b</v>
+        <v>obj_00128</v>
       </c>
       <c r="E2" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
@@ -3459,7 +3462,7 @@
       </c>
       <c r="F2" s="22">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>5.3785999999999999E-3</v>
+        <v>5.4136000000000011E-3</v>
       </c>
       <c r="G2" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -3467,14 +3470,14 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41943</v>
+        <v>42135</v>
       </c>
       <c r="I2" s="28">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42124</v>
+        <v>42319</v>
       </c>
       <c r="J2" s="18">
-        <v>0.99733989884720808</v>
+        <v>0.99727837976014466</v>
       </c>
       <c r="K2" s="23"/>
     </row>
@@ -3486,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21" t="str">
-        <v>obj_0011f</v>
+        <v>obj_00157</v>
       </c>
       <c r="E3" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -3494,7 +3497,7 @@
       </c>
       <c r="F3" s="22">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.3E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="G3" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -3502,14 +3505,14 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I3" s="28">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42311</v>
+        <v>42502</v>
       </c>
       <c r="J3" s="18">
-        <v>0.99566169873999066</v>
+        <v>0.99518544388735097</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -3521,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="str">
-        <v>obj_00125</v>
+        <v>obj_00166</v>
       </c>
       <c r="E4" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -3529,7 +3532,7 @@
       </c>
       <c r="F4" s="22">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>5.7000000000000002E-3</v>
+        <v>6.5000000000000006E-3</v>
       </c>
       <c r="G4" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -3537,14 +3540,14 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I4" s="28">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42493</v>
+        <v>42688</v>
       </c>
       <c r="J4" s="18">
-        <v>0.99144452267186178</v>
+        <v>0.99020156077964427</v>
       </c>
       <c r="K4" s="23"/>
     </row>
@@ -3556,7 +3559,7 @@
         <v>63</v>
       </c>
       <c r="D5" s="21" t="str">
-        <v>obj_00130</v>
+        <v>obj_00160</v>
       </c>
       <c r="E5" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -3564,7 +3567,7 @@
       </c>
       <c r="F5" s="22">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>7.4999999999999997E-3</v>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="G5" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -3572,14 +3575,14 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I5" s="28">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42677</v>
+        <v>42867</v>
       </c>
       <c r="J5" s="18">
-        <v>0.98502821458261403</v>
+        <v>0.98348239095329704</v>
       </c>
       <c r="K5" s="23"/>
     </row>
@@ -3587,7 +3590,7 @@
       <c r="A6" s="54"/>
       <c r="B6" s="54"/>
       <c r="D6" s="21" t="str">
-        <v>obj_0012d</v>
+        <v>obj_0015d</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -3595,7 +3598,7 @@
       </c>
       <c r="F6" s="22">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>1.1299999999999999E-2</v>
+        <v>1.14E-2</v>
       </c>
       <c r="G6" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -3603,20 +3606,20 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I6" s="28">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>43042</v>
+        <v>43234</v>
       </c>
       <c r="J6" s="18">
-        <v>0.96646292054688687</v>
+        <v>0.9661666072078946</v>
       </c>
       <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="21" t="str">
-        <v>obj_00126</v>
+        <v>obj_0015a</v>
       </c>
       <c r="E7" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -3624,7 +3627,7 @@
       </c>
       <c r="F7" s="22">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.4499999999999999E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="G7" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -3632,20 +3635,20 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I7" s="28">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>43409</v>
+        <v>43598</v>
       </c>
       <c r="J7" s="18">
-        <v>0.94309882368668019</v>
+        <v>0.94592267064079705</v>
       </c>
       <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="str">
-        <v>obj_00121</v>
+        <v>obj_0016c</v>
       </c>
       <c r="E8" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -3653,7 +3656,7 @@
       </c>
       <c r="F8" s="22">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1.7000000000000001E-2</v>
+        <v>1.5600000000000001E-2</v>
       </c>
       <c r="G8" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -3661,20 +3664,20 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I8" s="28">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>43773</v>
+        <v>43963</v>
       </c>
       <c r="J8" s="18">
-        <v>0.9175773083304064</v>
+        <v>0.92432436413541419</v>
       </c>
       <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="21" t="str">
-        <v>obj_00122</v>
+        <v>obj_00168</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -3682,7 +3685,7 @@
       </c>
       <c r="F9" s="22">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>2.0199999999999999E-2</v>
+        <v>1.8200000000000001E-2</v>
       </c>
       <c r="G9" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -3690,20 +3693,20 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I9" s="28">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>44503</v>
+        <v>44693</v>
       </c>
       <c r="J9" s="18">
-        <v>0.86617280980762246</v>
+        <v>0.87899113195046319</v>
       </c>
       <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="21" t="str">
-        <v>obj_00120</v>
+        <v>obj_0015f</v>
       </c>
       <c r="E10" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -3711,7 +3714,7 @@
       </c>
       <c r="F10" s="22">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>2.3E-2</v>
+        <v>2.06E-2</v>
       </c>
       <c r="G10" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -3719,20 +3722,20 @@
       </c>
       <c r="H10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I10" s="28">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>45600</v>
+        <v>45789</v>
       </c>
       <c r="J10" s="18">
-        <v>0.79059971098115767</v>
+        <v>0.81096864568402427</v>
       </c>
       <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="21" t="str">
-        <v>obj_00134</v>
+        <v>obj_00159</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -3740,7 +3743,7 @@
       </c>
       <c r="F11" s="22">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.4199999999999999E-2</v>
+        <v>2.1399999999999995E-2</v>
       </c>
       <c r="G11" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -3748,20 +3751,20 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I11" s="28">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>46329</v>
+        <v>46519</v>
       </c>
       <c r="J11" s="18">
-        <v>0.74277748536476151</v>
+        <v>0.76991953253976941</v>
       </c>
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="str">
-        <v>obj_00133</v>
+        <v>obj_00167</v>
       </c>
       <c r="E12" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -3769,7 +3772,7 @@
       </c>
       <c r="F12" s="22">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.5300000000000003E-2</v>
+        <v>2.2199999999999998E-2</v>
       </c>
       <c r="G12" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -3777,20 +3780,20 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I12" s="28">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>47427</v>
+        <v>47616</v>
       </c>
       <c r="J12" s="18">
-        <v>0.67729530569740715</v>
+        <v>0.71204963895355788</v>
       </c>
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="21" t="str">
-        <v>obj_00128</v>
+        <v>obj_00158</v>
       </c>
       <c r="E13" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -3798,7 +3801,7 @@
       </c>
       <c r="F13" s="22">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>2.6600000000000002E-2</v>
+        <v>2.35E-2</v>
       </c>
       <c r="G13" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -3806,14 +3809,14 @@
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41946</v>
+        <v>42136</v>
       </c>
       <c r="I13" s="28">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>49251</v>
+        <v>49443</v>
       </c>
       <c r="J13" s="18">
-        <v>0.57776018256954154</v>
+        <v>0.61733372763186234</v>
       </c>
       <c r="K13" s="23"/>
     </row>
@@ -7070,7 +7073,7 @@
       </c>
       <c r="E3" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00136#0001</v>
+        <v>obj_00121#0002</v>
       </c>
       <c r="F3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -7095,7 +7098,7 @@
       </c>
       <c r="E4" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013a#0001</v>
+        <v>obj_00127#0002</v>
       </c>
       <c r="F4" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E4)</f>
@@ -7120,7 +7123,7 @@
       </c>
       <c r="E5" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00139#0001</v>
+        <v>obj_00126#0002</v>
       </c>
       <c r="F5" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -7145,7 +7148,7 @@
       </c>
       <c r="E6" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013c#0001</v>
+        <v>obj_00129#0002</v>
       </c>
       <c r="F6" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -7170,7 +7173,7 @@
       </c>
       <c r="E7" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00138#0001</v>
+        <v>obj_00125#0002</v>
       </c>
       <c r="F7" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -7195,7 +7198,7 @@
       </c>
       <c r="E8" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013d#0001</v>
+        <v>obj_00122#0002</v>
       </c>
       <c r="F8" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -7220,7 +7223,7 @@
       </c>
       <c r="E9" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013b#0001</v>
+        <v>obj_00128#0002</v>
       </c>
       <c r="F9" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -7245,7 +7248,7 @@
       </c>
       <c r="E10" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0013e#0001</v>
+        <v>obj_00124#0002</v>
       </c>
       <c r="F10" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -7270,7 +7273,7 @@
       </c>
       <c r="E11" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00137#0001</v>
+        <v>obj_00123#0002</v>
       </c>
       <c r="F11" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -7302,35 +7305,36 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.7109375" style="3" customWidth="1"/>
-    <col min="13" max="14" width="2.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="3" customWidth="1"/>
+    <col min="14" max="15" width="2.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="55"/>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -7343,9 +7347,10 @@
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
-    </row>
-    <row r="2" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="56"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -7354,71 +7359,75 @@
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
       <c r="H2" s="48"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="48"/>
+      <c r="J2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="6" t="str">
+      <c r="K2" s="6" t="str">
         <f>Currency&amp;"_YC"&amp;"STDRH"</f>
         <v>HKD_YCSTDRH</v>
       </c>
-      <c r="K2" s="58" t="str">
-        <f>J2&amp;"_Swaps.xml"</f>
+      <c r="L2" s="58" t="str">
+        <f>K2&amp;"_Swaps.xml"</f>
         <v>HKD_YCSTDRH_Swaps.xml</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="59"/>
-    </row>
-    <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="48"/>
+      <c r="N2" s="59"/>
+    </row>
+    <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="H3" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="I3" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="J3" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="K3" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="60" t="str">
-        <f>IF(Serialize,_xll.ohObjectSave(K4:K28,SerializationPath&amp;K2,FileOverwrite,,Serialize),"---")</f>
+      <c r="L3" s="60" t="str">
+        <f>IF(Serialize,_xll.ohObjectSave(L4:L28,SerializationPath&amp;L2,FileOverwrite,,Serialize),"---")</f>
         <v>---</v>
       </c>
-      <c r="L3" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K3)</f>
+      <c r="M3" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L3)</f>
         <v/>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="N3" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="62" t="s">
+      <c r="P3" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="62" t="s">
+      <c r="Q3" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="62" t="s">
+      <c r="R3" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="62" t="s">
+      <c r="S3" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="62" t="s">
+      <c r="T3" s="62" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48"/>
       <c r="C4" s="48"/>
@@ -7429,34 +7438,35 @@
       <c r="H4" s="48"/>
       <c r="I4" s="48"/>
       <c r="J4" s="48"/>
-      <c r="K4" s="63" t="str">
-        <f>_xll.qlIborIndex(,FamilyName,I2,O4,Currency,P4,Q4,R4,S4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0011e#0001</v>
-      </c>
-      <c r="L4" s="64" t="str">
-        <f>_xll.ohRangeRetrieveError(K4)</f>
+      <c r="K4" s="48"/>
+      <c r="L4" s="63" t="str">
+        <f>_xll.qlIborIndex(,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>obj_00120#0003</v>
+      </c>
+      <c r="M4" s="64" t="str">
+        <f>_xll.ohRangeRetrieveError(L4)</f>
         <v/>
       </c>
-      <c r="M4" s="76" t="s">
+      <c r="N4" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="O4" s="65">
-        <v>0</v>
-      </c>
-      <c r="P4" s="65" t="s">
+      <c r="P4" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" s="65" t="s">
+      <c r="R4" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="R4" s="65" t="b">
+      <c r="S4" s="65" t="b">
         <v>1</v>
       </c>
-      <c r="S4" s="65" t="s">
+      <c r="T4" s="65" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
@@ -7469,1000 +7479,1070 @@
       <c r="J5" s="48"/>
       <c r="K5" s="48"/>
       <c r="L5" s="48"/>
-      <c r="M5" s="76" t="s">
+      <c r="M5" s="48"/>
+      <c r="N5" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
       <c r="B6" s="66">
         <v>1</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66">
+        <v>0</v>
+      </c>
+      <c r="D6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="E6" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="F6" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="G6" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="H6" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="68" t="str">
-        <f t="shared" ref="H6:H28" si="0">IF(UPPER(RIGHT($D6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($D6))="M",MoneyMarketDayCounter,"--"))</f>
+      <c r="I6" s="68" t="str">
+        <f t="shared" ref="I6:I28" si="0">IF(UPPER(RIGHT($E6))="B",BondBasisDayCounter,IF(UPPER(RIGHT($E6))="M",MoneyMarketDayCounter,"--"))</f>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I6" s="69">
-        <v>0</v>
-      </c>
-      <c r="J6" s="70" t="str">
-        <f t="shared" ref="J6:J28" si="1">Currency&amp;$D6&amp;$E6&amp;$C6&amp;QuoteSuffix</f>
+      <c r="J6" s="69">
+        <v>0</v>
+      </c>
+      <c r="K6" s="70" t="str">
+        <f t="shared" ref="K6:K28" si="1">Currency&amp;$E6&amp;$F6&amp;$D6&amp;QuoteSuffix</f>
         <v>HKDQM3H1Y_Quote</v>
       </c>
-      <c r="K6" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J6,$C6,Calendar,$F6,$G6,$H6,$K$4,$I6,B6&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0011f#0001</v>
-      </c>
-      <c r="L6" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K6)</f>
+      <c r="L6" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K6,$B6,$D6,Calendar,$G6,$H6,$I6,$L$4,$J6,C6&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00157#0003</v>
+      </c>
+      <c r="M6" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L6)</f>
         <v/>
       </c>
-      <c r="M6" s="76" t="s">
+      <c r="N6" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
       <c r="B7" s="66">
         <v>1</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="66">
+        <v>0</v>
+      </c>
+      <c r="D7" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="E7" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="F7" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="G7" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="H7" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="72" t="str">
+      <c r="I7" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I7" s="69">
-        <v>0</v>
-      </c>
-      <c r="J7" s="73" t="str">
+      <c r="J7" s="69">
+        <v>0</v>
+      </c>
+      <c r="K7" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H15M_Quote</v>
       </c>
-      <c r="K7" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J7,$C7,Calendar,$F7,$G7,$H7,$K$4,$I7,B7&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00132#0001</v>
-      </c>
-      <c r="L7" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K7)</f>
+      <c r="L7" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K7,$B7,$D7,Calendar,$G7,$H7,$I7,$L$4,$J7,C7&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00169#0003</v>
+      </c>
+      <c r="M7" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L7)</f>
         <v/>
       </c>
-      <c r="M7" s="76" t="s">
+      <c r="N7" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41"/>
       <c r="B8" s="66">
         <v>1</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="66">
+        <v>0</v>
+      </c>
+      <c r="D8" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="E8" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="67" t="s">
+      <c r="F8" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="G8" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="H8" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="72" t="str">
+      <c r="I8" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I8" s="69">
-        <v>0</v>
-      </c>
-      <c r="J8" s="73" t="str">
+      <c r="J8" s="69">
+        <v>0</v>
+      </c>
+      <c r="K8" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H18M_Quote</v>
       </c>
-      <c r="K8" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J8,$C8,Calendar,$F8,$G8,$H8,$K$4,$I8,B8&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00125#0001</v>
-      </c>
-      <c r="L8" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K8)</f>
+      <c r="L8" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K8,$B8,$D8,Calendar,$G8,$H8,$I8,$L$4,$J8,C8&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00166#0003</v>
+      </c>
+      <c r="M8" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L8)</f>
         <v/>
       </c>
-      <c r="M8" s="76" t="s">
+      <c r="N8" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
       <c r="B9" s="66">
         <v>1</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="66">
+        <v>0</v>
+      </c>
+      <c r="D9" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="E9" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="F9" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="G9" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="72" t="s">
+      <c r="H9" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="72" t="str">
+      <c r="I9" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I9" s="69">
-        <v>0</v>
-      </c>
-      <c r="J9" s="73" t="str">
+      <c r="J9" s="69">
+        <v>0</v>
+      </c>
+      <c r="K9" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H21M_Quote</v>
       </c>
-      <c r="K9" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J9,$C9,Calendar,$F9,$G9,$H9,$K$4,$I9,B9&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00123#0001</v>
-      </c>
-      <c r="L9" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K9)</f>
+      <c r="L9" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K9,$B9,$D9,Calendar,$G9,$H9,$I9,$L$4,$J9,C9&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00163#0003</v>
+      </c>
+      <c r="M9" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L9)</f>
         <v/>
       </c>
-      <c r="M9" s="76" t="s">
+      <c r="N9" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="41"/>
       <c r="B10" s="66">
         <v>1</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="66">
+        <v>0</v>
+      </c>
+      <c r="D10" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="E10" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="F10" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="G10" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="72" t="s">
+      <c r="H10" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="72" t="str">
+      <c r="I10" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I10" s="69">
-        <v>0</v>
-      </c>
-      <c r="J10" s="73" t="str">
+      <c r="J10" s="69">
+        <v>0</v>
+      </c>
+      <c r="K10" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H2Y_Quote</v>
       </c>
-      <c r="K10" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J10,$C10,Calendar,$F10,$G10,$H10,$K$4,$I10,B10&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00130#0001</v>
-      </c>
-      <c r="L10" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K10)</f>
+      <c r="L10" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K10,$B10,$D10,Calendar,$G10,$H10,$I10,$L$4,$J10,C10&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00160#0003</v>
+      </c>
+      <c r="M10" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L10)</f>
         <v/>
       </c>
-      <c r="M10" s="76" t="s">
+      <c r="N10" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="41"/>
       <c r="B11" s="66">
         <v>1</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="66">
+        <v>0</v>
+      </c>
+      <c r="D11" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="E11" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="F11" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="68" t="s">
+      <c r="G11" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="H11" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="72" t="str">
+      <c r="I11" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I11" s="69">
-        <v>0</v>
-      </c>
-      <c r="J11" s="73" t="str">
+      <c r="J11" s="69">
+        <v>0</v>
+      </c>
+      <c r="K11" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H3Y_Quote</v>
       </c>
-      <c r="K11" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J11,$C11,Calendar,$F11,$G11,$H11,$K$4,$I11,B11&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012d#0001</v>
-      </c>
-      <c r="L11" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K11)</f>
+      <c r="L11" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K11,$B11,$D11,Calendar,$G11,$H11,$I11,$L$4,$J11,C11&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015d#0003</v>
+      </c>
+      <c r="M11" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L11)</f>
         <v/>
       </c>
-      <c r="M11" s="76" t="s">
+      <c r="N11" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="41"/>
       <c r="B12" s="66">
         <v>1</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="66">
+        <v>0</v>
+      </c>
+      <c r="D12" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="E12" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="F12" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="G12" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="72" t="s">
+      <c r="H12" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="72" t="str">
+      <c r="I12" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I12" s="69">
-        <v>0</v>
-      </c>
-      <c r="J12" s="73" t="str">
+      <c r="J12" s="69">
+        <v>0</v>
+      </c>
+      <c r="K12" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H4Y_Quote</v>
       </c>
-      <c r="K12" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J12,$C12,Calendar,$F12,$G12,$H12,$K$4,$I12,B12&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00126#0001</v>
-      </c>
-      <c r="L12" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K12)</f>
+      <c r="L12" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K12,$B12,$D12,Calendar,$G12,$H12,$I12,$L$4,$J12,C12&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015a#0003</v>
+      </c>
+      <c r="M12" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L12)</f>
         <v/>
       </c>
-      <c r="M12" s="76" t="s">
+      <c r="N12" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="41"/>
       <c r="B13" s="66">
         <v>1</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66">
+        <v>0</v>
+      </c>
+      <c r="D13" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="E13" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="F13" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="G13" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="H13" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="72" t="str">
+      <c r="I13" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I13" s="69">
-        <v>0</v>
-      </c>
-      <c r="J13" s="73" t="str">
+      <c r="J13" s="69">
+        <v>0</v>
+      </c>
+      <c r="K13" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H5Y_Quote</v>
       </c>
-      <c r="K13" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J13,$C13,Calendar,$F13,$G13,$H13,$K$4,$I13,B13&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00121#0001</v>
-      </c>
-      <c r="L13" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K13)</f>
+      <c r="L13" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K13,$B13,$D13,Calendar,$G13,$H13,$I13,$L$4,$J13,C13&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0016c#0003</v>
+      </c>
+      <c r="M13" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L13)</f>
         <v/>
       </c>
-      <c r="M13" s="76" t="s">
+      <c r="N13" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="41"/>
       <c r="B14" s="66">
         <v>1</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="66">
+        <v>0</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="E14" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="F14" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="G14" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="H14" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="72" t="str">
+      <c r="I14" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I14" s="69">
-        <v>0</v>
-      </c>
-      <c r="J14" s="73" t="str">
+      <c r="J14" s="69">
+        <v>0</v>
+      </c>
+      <c r="K14" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H6Y_Quote</v>
       </c>
-      <c r="K14" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J14,$C14,Calendar,$F14,$G14,$H14,$K$4,$I14,B14&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012f#0001</v>
-      </c>
-      <c r="L14" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K14)</f>
+      <c r="L14" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K14,$B14,$D14,Calendar,$G14,$H14,$I14,$L$4,$J14,C14&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0016a#0003</v>
+      </c>
+      <c r="M14" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L14)</f>
         <v/>
       </c>
-      <c r="M14" s="76" t="s">
+      <c r="N14" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="41"/>
       <c r="B15" s="66">
         <v>1</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="66">
+        <v>0</v>
+      </c>
+      <c r="D15" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="E15" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="F15" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="68" t="s">
+      <c r="G15" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="H15" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H15" s="72" t="str">
+      <c r="I15" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I15" s="69">
-        <v>0</v>
-      </c>
-      <c r="J15" s="73" t="str">
+      <c r="J15" s="69">
+        <v>0</v>
+      </c>
+      <c r="K15" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H7Y_Quote</v>
       </c>
-      <c r="K15" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J15,$C15,Calendar,$F15,$G15,$H15,$K$4,$I15,B15&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00122#0001</v>
-      </c>
-      <c r="L15" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K15)</f>
+      <c r="L15" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K15,$B15,$D15,Calendar,$G15,$H15,$I15,$L$4,$J15,C15&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00168#0003</v>
+      </c>
+      <c r="M15" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L15)</f>
         <v/>
       </c>
-      <c r="M15" s="76" t="s">
+      <c r="N15" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="41"/>
       <c r="B16" s="66">
         <v>1</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="66">
+        <v>0</v>
+      </c>
+      <c r="D16" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="E16" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="F16" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="G16" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="H16" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="72" t="str">
+      <c r="I16" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I16" s="69">
-        <v>0</v>
-      </c>
-      <c r="J16" s="73" t="str">
+      <c r="J16" s="69">
+        <v>0</v>
+      </c>
+      <c r="K16" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H8Y_Quote</v>
       </c>
-      <c r="K16" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J16,$C16,Calendar,$F16,$G16,$H16,$K$4,$I16,B16&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00129#0001</v>
-      </c>
-      <c r="L16" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K16)</f>
+      <c r="L16" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K16,$B16,$D16,Calendar,$G16,$H16,$I16,$L$4,$J16,C16&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00165#0003</v>
+      </c>
+      <c r="M16" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L16)</f>
         <v/>
       </c>
-      <c r="M16" s="76" t="s">
+      <c r="N16" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41"/>
       <c r="B17" s="66">
         <v>1</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="66">
+        <v>0</v>
+      </c>
+      <c r="D17" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="E17" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="67" t="s">
+      <c r="F17" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="G17" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="72" t="s">
+      <c r="H17" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="72" t="str">
+      <c r="I17" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I17" s="69">
-        <v>0</v>
-      </c>
-      <c r="J17" s="73" t="str">
+      <c r="J17" s="69">
+        <v>0</v>
+      </c>
+      <c r="K17" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H9Y_Quote</v>
       </c>
-      <c r="K17" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J17,$C17,Calendar,$F17,$G17,$H17,$K$4,$I17,B17&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012b#0001</v>
-      </c>
-      <c r="L17" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K17)</f>
+      <c r="L17" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K17,$B17,$D17,Calendar,$G17,$H17,$I17,$L$4,$J17,C17&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00162#0003</v>
+      </c>
+      <c r="M17" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L17)</f>
         <v/>
       </c>
-      <c r="M17" s="76" t="s">
+      <c r="N17" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41"/>
       <c r="B18" s="66">
         <v>1</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="66">
+        <v>0</v>
+      </c>
+      <c r="D18" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="67" t="s">
+      <c r="E18" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="F18" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="G18" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="H18" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="72" t="str">
+      <c r="I18" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I18" s="69">
-        <v>0</v>
-      </c>
-      <c r="J18" s="73" t="str">
+      <c r="J18" s="69">
+        <v>0</v>
+      </c>
+      <c r="K18" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H10Y_Quote</v>
       </c>
-      <c r="K18" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J18,$C18,Calendar,$F18,$G18,$H18,$K$4,$I18,B18&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00120#0001</v>
-      </c>
-      <c r="L18" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K18)</f>
+      <c r="L18" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K18,$B18,$D18,Calendar,$G18,$H18,$I18,$L$4,$J18,C18&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015f#0003</v>
+      </c>
+      <c r="M18" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L18)</f>
         <v/>
       </c>
-      <c r="M18" s="76" t="s">
+      <c r="N18" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41"/>
       <c r="B19" s="66">
         <v>1</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66">
+        <v>0</v>
+      </c>
+      <c r="D19" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="67" t="s">
+      <c r="E19" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="F19" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="68" t="s">
+      <c r="G19" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="72" t="s">
+      <c r="H19" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="72" t="str">
+      <c r="I19" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I19" s="69">
-        <v>0</v>
-      </c>
-      <c r="J19" s="73" t="str">
+      <c r="J19" s="69">
+        <v>0</v>
+      </c>
+      <c r="K19" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H11Y_Quote</v>
       </c>
-      <c r="K19" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J19,$C19,Calendar,$F19,$G19,$H19,$K$4,$I19,B19&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00124#0001</v>
-      </c>
-      <c r="L19" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K19)</f>
+      <c r="L19" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K19,$B19,$D19,Calendar,$G19,$H19,$I19,$L$4,$J19,C19&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015c#0003</v>
+      </c>
+      <c r="M19" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L19)</f>
         <v/>
       </c>
-      <c r="M19" s="76" t="s">
+      <c r="N19" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41"/>
       <c r="B20" s="66">
         <v>1</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="66">
+        <v>0</v>
+      </c>
+      <c r="D20" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="67" t="s">
+      <c r="E20" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="67" t="s">
+      <c r="F20" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="68" t="s">
+      <c r="G20" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="72" t="s">
+      <c r="H20" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="72" t="str">
+      <c r="I20" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I20" s="69">
-        <v>0</v>
-      </c>
-      <c r="J20" s="73" t="str">
+      <c r="J20" s="69">
+        <v>0</v>
+      </c>
+      <c r="K20" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H12Y_Quote</v>
       </c>
-      <c r="K20" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J20,$C20,Calendar,$F20,$G20,$H20,$K$4,$I20,B20&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00134#0001</v>
-      </c>
-      <c r="L20" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K20)</f>
+      <c r="L20" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K20,$B20,$D20,Calendar,$G20,$H20,$I20,$L$4,$J20,C20&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00159#0003</v>
+      </c>
+      <c r="M20" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L20)</f>
         <v/>
       </c>
-      <c r="M20" s="76" t="s">
+      <c r="N20" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41"/>
       <c r="B21" s="66">
         <v>1</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66">
+        <v>0</v>
+      </c>
+      <c r="D21" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="67" t="s">
+      <c r="E21" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="F21" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="G21" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="72" t="s">
+      <c r="H21" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="72" t="str">
+      <c r="I21" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I21" s="69">
-        <v>0</v>
-      </c>
-      <c r="J21" s="73" t="str">
+      <c r="J21" s="69">
+        <v>0</v>
+      </c>
+      <c r="K21" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H13Y_Quote</v>
       </c>
-      <c r="K21" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J21,$C21,Calendar,$F21,$G21,$H21,$K$4,$I21,B21&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012e#0001</v>
-      </c>
-      <c r="L21" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K21)</f>
+      <c r="L21" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K21,$B21,$D21,Calendar,$G21,$H21,$I21,$L$4,$J21,C21&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0016b#0003</v>
+      </c>
+      <c r="M21" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L21)</f>
         <v/>
       </c>
-      <c r="M21" s="76" t="s">
+      <c r="N21" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41"/>
       <c r="B22" s="66">
         <v>1</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66">
+        <v>0</v>
+      </c>
+      <c r="D22" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="E22" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="67" t="s">
+      <c r="F22" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="G22" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="72" t="s">
+      <c r="H22" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H22" s="72" t="str">
+      <c r="I22" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I22" s="69">
-        <v>0</v>
-      </c>
-      <c r="J22" s="73" t="str">
+      <c r="J22" s="69">
+        <v>0</v>
+      </c>
+      <c r="K22" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H14Y_Quote</v>
       </c>
-      <c r="K22" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J22,$C22,Calendar,$F22,$G22,$H22,$K$4,$I22,B22&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012c#0001</v>
-      </c>
-      <c r="L22" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K22)</f>
+      <c r="L22" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K22,$B22,$D22,Calendar,$G22,$H22,$I22,$L$4,$J22,C22&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0016d#0003</v>
+      </c>
+      <c r="M22" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L22)</f>
         <v/>
       </c>
-      <c r="M22" s="76" t="s">
+      <c r="N22" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41"/>
       <c r="B23" s="66">
         <v>1</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="66">
+        <v>0</v>
+      </c>
+      <c r="D23" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="67" t="s">
+      <c r="E23" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="67" t="s">
+      <c r="F23" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="G23" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="72" t="s">
+      <c r="H23" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="72" t="str">
+      <c r="I23" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I23" s="69">
-        <v>0</v>
-      </c>
-      <c r="J23" s="73" t="str">
+      <c r="J23" s="69">
+        <v>0</v>
+      </c>
+      <c r="K23" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H15Y_Quote</v>
       </c>
-      <c r="K23" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J23,$C23,Calendar,$F23,$G23,$H23,$K$4,$I23,B23&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00133#0001</v>
-      </c>
-      <c r="L23" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K23)</f>
+      <c r="L23" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K23,$B23,$D23,Calendar,$G23,$H23,$I23,$L$4,$J23,C23&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00167#0003</v>
+      </c>
+      <c r="M23" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L23)</f>
         <v/>
       </c>
-      <c r="M23" s="76" t="s">
+      <c r="N23" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41"/>
       <c r="B24" s="66">
         <v>1</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66">
+        <v>0</v>
+      </c>
+      <c r="D24" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="E24" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="67" t="s">
+      <c r="F24" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="G24" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G24" s="72" t="s">
+      <c r="H24" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="72" t="str">
+      <c r="I24" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I24" s="69">
-        <v>0</v>
-      </c>
-      <c r="J24" s="73" t="str">
+      <c r="J24" s="69">
+        <v>0</v>
+      </c>
+      <c r="K24" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H16Y_Quote</v>
       </c>
-      <c r="K24" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J24,$C24,Calendar,$F24,$G24,$H24,$K$4,$I24,B24&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00135#0001</v>
-      </c>
-      <c r="L24" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K24)</f>
+      <c r="L24" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K24,$B24,$D24,Calendar,$G24,$H24,$I24,$L$4,$J24,C24&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00164#0003</v>
+      </c>
+      <c r="M24" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L24)</f>
         <v/>
       </c>
-      <c r="M24" s="76" t="s">
+      <c r="N24" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41"/>
       <c r="B25" s="66">
         <v>1</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66">
+        <v>0</v>
+      </c>
+      <c r="D25" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="E25" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="67" t="s">
+      <c r="F25" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="G25" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="72" t="s">
+      <c r="H25" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="72" t="str">
+      <c r="I25" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I25" s="69">
-        <v>0</v>
-      </c>
-      <c r="J25" s="73" t="str">
+      <c r="J25" s="69">
+        <v>0</v>
+      </c>
+      <c r="K25" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H17Y_Quote</v>
       </c>
-      <c r="K25" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J25,$C25,Calendar,$F25,$G25,$H25,$K$4,$I25,B25&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00131#0001</v>
-      </c>
-      <c r="L25" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K25)</f>
+      <c r="L25" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K25,$B25,$D25,Calendar,$G25,$H25,$I25,$L$4,$J25,C25&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00161#0003</v>
+      </c>
+      <c r="M25" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L25)</f>
         <v/>
       </c>
-      <c r="M25" s="76" t="s">
+      <c r="N25" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41"/>
       <c r="B26" s="66">
         <v>1</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66">
+        <v>0</v>
+      </c>
+      <c r="D26" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="67" t="s">
+      <c r="E26" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="67" t="s">
+      <c r="F26" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="68" t="s">
+      <c r="G26" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="72" t="s">
+      <c r="H26" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="72" t="str">
+      <c r="I26" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I26" s="69">
-        <v>0</v>
-      </c>
-      <c r="J26" s="73" t="str">
+      <c r="J26" s="69">
+        <v>0</v>
+      </c>
+      <c r="K26" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H18Y_Quote</v>
       </c>
-      <c r="K26" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J26,$C26,Calendar,$F26,$G26,$H26,$K$4,$I26,B26&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00127#0001</v>
-      </c>
-      <c r="L26" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K26)</f>
+      <c r="L26" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K26,$B26,$D26,Calendar,$G26,$H26,$I26,$L$4,$J26,C26&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015e#0003</v>
+      </c>
+      <c r="M26" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L26)</f>
         <v/>
       </c>
-      <c r="M26" s="76" t="s">
+      <c r="N26" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="41"/>
       <c r="B27" s="66">
         <v>1</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="66">
+        <v>0</v>
+      </c>
+      <c r="D27" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="67" t="s">
+      <c r="E27" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="67" t="s">
+      <c r="F27" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="68" t="s">
+      <c r="G27" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="72" t="s">
+      <c r="H27" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="72" t="str">
+      <c r="I27" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I27" s="69">
-        <v>0</v>
-      </c>
-      <c r="J27" s="73" t="str">
+      <c r="J27" s="69">
+        <v>0</v>
+      </c>
+      <c r="K27" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H19Y_Quote</v>
       </c>
-      <c r="K27" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J27,$C27,Calendar,$F27,$G27,$H27,$K$4,$I27,B27&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0012a#0001</v>
-      </c>
-      <c r="L27" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K27)</f>
+      <c r="L27" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K27,$B27,$D27,Calendar,$G27,$H27,$I27,$L$4,$J27,C27&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_0015b#0003</v>
+      </c>
+      <c r="M27" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L27)</f>
         <v/>
       </c>
-      <c r="M27" s="76" t="s">
+      <c r="N27" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="41"/>
       <c r="B28" s="66">
         <v>1</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="66">
+        <v>0</v>
+      </c>
+      <c r="D28" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="67" t="s">
+      <c r="E28" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="F28" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="68" t="s">
+      <c r="G28" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="H28" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="H28" s="72" t="str">
+      <c r="I28" s="72" t="str">
         <f t="shared" si="0"/>
         <v>Actual/365 (Fixed)</v>
       </c>
-      <c r="I28" s="69">
-        <v>0</v>
-      </c>
-      <c r="J28" s="73" t="str">
+      <c r="J28" s="69">
+        <v>0</v>
+      </c>
+      <c r="K28" s="73" t="str">
         <f t="shared" si="1"/>
         <v>HKDQM3H20Y_Quote</v>
       </c>
-      <c r="K28" s="71" t="str">
-        <f>_xll.qlSwapRateHelper2(,$J28,$C28,Calendar,$F28,$G28,$H28,$K$4,$I28,B28&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00128#0001</v>
-      </c>
-      <c r="L28" s="61" t="str">
-        <f>_xll.ohRangeRetrieveError(K28)</f>
+      <c r="L28" s="71" t="str">
+        <f>_xll.qlSwapRateHelper2(,$K28,$B28,$D28,Calendar,$G28,$H28,$I28,$L$4,$J28,C28&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
+        <v>obj_00158#0003</v>
+      </c>
+      <c r="M28" s="61" t="str">
+        <f>_xll.ohRangeRetrieveError(L28)</f>
         <v/>
       </c>
-      <c r="M28" s="76" t="s">
+      <c r="N28" s="76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -8473,22 +8553,23 @@
       <c r="H29" s="33"/>
       <c r="I29" s="33"/>
       <c r="J29" s="33"/>
-      <c r="K29" s="74"/>
+      <c r="K29" s="33"/>
       <c r="L29" s="74"/>
-      <c r="M29" s="75"/>
+      <c r="M29" s="74"/>
+      <c r="N29" s="75"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T4">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R4">
       <formula1>"Following,Modified Following,Preceding,Modified Preceding,Unadjusted"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G28">
       <formula1>"Annual,Semiannual,EveryFourthMonth,Quarterly,Bimonthly,Monthly,Biweekly,Weekly,Daily,Once,NoFrequency"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H28">
       <formula1>"Following,Modified Following,Preceding,Modified Preceding,Month End Reference,Unadjusted Month End,Unadjusted"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
use Deposits instead of LastFixing Quotes in HKD curves
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_YCSTDBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="555" windowWidth="19440" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19125" windowHeight="12255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1792,7 +1792,7 @@
     <row r="1" spans="2:10" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="77" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - May  5 2015 15:27:06</v>
+        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - Jul 20 2015 13:11:27</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D14" s="102" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,_xll.ohPack(Selected!D2:D126),,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>HKDYCSTD#0008</v>
+        <v>HKDYCSTD#0005</v>
       </c>
       <c r="E14" s="80"/>
       <c r="F14" s="122"/>
@@ -2117,7 +2117,7 @@
       <c r="B23" s="78"/>
       <c r="C23" s="113">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="D23" s="114">
         <f>MAX(_xll.ohPack(Selected!J1:J126))</f>
@@ -2130,11 +2130,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="115">
         <f>MAX(_xll.ohPack(Selected!I2:I126))</f>
-        <v>49443</v>
+        <v>49486</v>
       </c>
       <c r="D24" s="90">
         <f>MIN(_xll.ohPack(Selected!J1:J126))</f>
-        <v>0.61733372763186234</v>
+        <v>0.59816766612848471</v>
       </c>
       <c r="E24" s="80"/>
       <c r="F24" s="122"/>
@@ -2223,7 +2223,7 @@
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="10" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
@@ -2263,15 +2263,15 @@
     <row r="2" spans="1:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>Deposits!E3</f>
-        <v>obj_00121#0002</v>
+        <v>obj_00138#0005</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A2)</f>
-        <v>HkdHiborONLastFixing_Quote</v>
+        <v>HKDOND_Quote</v>
       </c>
       <c r="C2" s="5">
         <f>_xll.qlRateHelperQuoteValue($A2,Trigger)</f>
-        <v>4.7990000000000006E-4</v>
+        <v>5.6530000000000003E-4</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="b">
@@ -2285,25 +2285,25 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($A2,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I2" s="12">
         <f>_xll.qlRateHelperLatestDate($A2,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
         <f>Deposits!E4</f>
-        <v>obj_00127#0002</v>
+        <v>obj_0013f#0003</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A3)</f>
-        <v>HkdHiborSWLastFixing_Quote</v>
-      </c>
-      <c r="C3" s="5">
+        <v>HKDSWD_Quote</v>
+      </c>
+      <c r="C3" s="5" t="e">
         <f>_xll.qlRateHelperQuoteValue($A3,Trigger)</f>
-        <v>9.9140000000000014E-4</v>
+        <v>#NUM!</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="b">
@@ -2317,25 +2317,25 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($A3,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I3" s="12">
         <f>_xll.qlRateHelperLatestDate($A3,Trigger)</f>
-        <v>42142</v>
+        <v>42187</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="str">
         <f>Deposits!E5</f>
-        <v>obj_00126#0002</v>
+        <v>obj_0013e#0003</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A4)</f>
-        <v>HkdHibor2WLastFixing_Quote</v>
+        <v>HKD2WD_Quote</v>
       </c>
       <c r="C4" s="5">
         <f>_xll.qlRateHelperQuoteValue($A4,Trigger)</f>
-        <v>1.3820000000000002E-3</v>
+        <v>1.6257000000000001E-3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="b">
@@ -2349,25 +2349,25 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($A4,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I4" s="12">
         <f>_xll.qlRateHelperLatestDate($A4,Trigger)</f>
-        <v>42150</v>
+        <v>42194</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="str">
         <f>Deposits!E6</f>
-        <v>obj_00129#0002</v>
+        <v>obj_00139#0003</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A5)</f>
-        <v>HkdHibor1MLastFixing_Quote</v>
+        <v>HKD1MD_Quote</v>
       </c>
       <c r="C5" s="5">
         <f>_xll.qlRateHelperQuoteValue($A5,Trigger)</f>
-        <v>2.4043000000000003E-3</v>
+        <v>2.4094000000000003E-3</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="b">
@@ -2381,25 +2381,25 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($A5,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I5" s="12">
         <f>_xll.qlRateHelperLatestDate($A5,Trigger)</f>
-        <v>42166</v>
+        <v>42212</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>Deposits!E7</f>
-        <v>obj_00125#0002</v>
+        <v>obj_0013d#0003</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A6)</f>
-        <v>HkdHibor2MLastFixing_Quote</v>
+        <v>HKD2MD_Quote</v>
       </c>
       <c r="C6" s="5">
         <f>_xll.qlRateHelperQuoteValue($A6,Trigger)</f>
-        <v>3.0371000000000005E-3</v>
+        <v>3.0586000000000003E-3</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="b">
@@ -2413,25 +2413,25 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($A6,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I6" s="12">
         <f>_xll.qlRateHelperLatestDate($A6,Trigger)</f>
-        <v>42198</v>
+        <v>42241</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="str">
         <f>Deposits!E8</f>
-        <v>obj_00122#0002</v>
+        <v>obj_0013a#0003</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A7)</f>
-        <v>HkdHibor3MLastFixing_Quote</v>
+        <v>HKD3MD_Quote</v>
       </c>
       <c r="C7" s="5">
         <f>_xll.qlRateHelperQuoteValue($A7,Trigger)</f>
-        <v>3.8600000000000001E-3</v>
+        <v>3.8814000000000006E-3</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="b">
@@ -2445,25 +2445,25 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($A7,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I7" s="12">
         <f>_xll.qlRateHelperLatestDate($A7,Trigger)</f>
-        <v>42227</v>
+        <v>42272</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="str">
         <f>Deposits!E9</f>
-        <v>obj_00128#0002</v>
+        <v>obj_00140#0003</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A8)</f>
-        <v>HkdHibor6MLastFixing_Quote</v>
+        <v>HKD6MD_Quote</v>
       </c>
       <c r="C8" s="5">
         <f>_xll.qlRateHelperQuoteValue($A8,Trigger)</f>
-        <v>5.4136000000000011E-3</v>
+        <v>5.4286000000000004E-3</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="b">
@@ -2477,21 +2477,21 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($A8,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I8" s="12">
         <f>_xll.qlRateHelperLatestDate($A8,Trigger)</f>
-        <v>42319</v>
+        <v>42366</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="str">
         <f>Deposits!E10</f>
-        <v>obj_00124#0002</v>
+        <v>obj_0013c#0003</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A9)</f>
-        <v>HkdHibor9MLastFixing_Quote</v>
+        <v>HKD9MD_Quote</v>
       </c>
       <c r="C9" s="5" t="e">
         <f>_xll.qlRateHelperQuoteValue($A9,Trigger)</f>
@@ -2509,25 +2509,25 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($A9,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I9" s="12">
         <f>_xll.qlRateHelperLatestDate($A9,Trigger)</f>
-        <v>42411</v>
+        <v>42458</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>Deposits!E11</f>
-        <v>obj_00123#0002</v>
+        <v>obj_0013b#0003</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>_xll.qlRateHelperQuoteName(A10)</f>
-        <v>HkdHibor1YLastFixing_Quote</v>
+        <v>HKD1YD_Quote</v>
       </c>
       <c r="C10" s="8">
         <f>_xll.qlRateHelperQuoteValue($A10,Trigger)</f>
-        <v>8.4153000000000006E-3</v>
+        <v>8.4329000000000001E-3</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="9" t="b">
@@ -2541,17 +2541,17 @@
       </c>
       <c r="H10" s="13">
         <f>_xll.qlRateHelperEarliestDate($A10,Trigger)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I10" s="14">
         <f>_xll.qlRateHelperLatestDate($A10,Trigger)</f>
-        <v>42501</v>
+        <v>42548</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f>Swaps!L6</f>
-        <v>obj_00157#0003</v>
+        <v>obj_00127#0001</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A11)</f>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="C11" s="5">
         <f>_xll.qlRateHelperQuoteValue($A11,Trigger)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="D11" s="5">
         <f>_xll.qlSwapRateHelperSpread($A11,Trigger)</f>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($A11,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I11" s="12">
         <f>_xll.qlRateHelperLatestDate($A11,Trigger)</f>
-        <v>42502</v>
+        <v>42548</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>Swaps!L7</f>
-        <v>obj_00169#0003</v>
+        <v>obj_00130#0001</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A12)</f>
@@ -2613,17 +2613,17 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($A12,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I12" s="12">
         <f>_xll.qlRateHelperLatestDate($A12,Trigger)</f>
-        <v>42594</v>
+        <v>42639</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>Swaps!L8</f>
-        <v>obj_00166#0003</v>
+        <v>obj_00128#0001</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A13)</f>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="C13" s="5">
         <f>_xll.qlRateHelperQuoteValue($A13,Trigger)</f>
-        <v>6.5000000000000006E-3</v>
+        <v>6.6999999999999994E-3</v>
       </c>
       <c r="D13" s="5">
         <f>_xll.qlSwapRateHelperSpread($A13,Trigger)</f>
@@ -2649,17 +2649,17 @@
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($A13,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I13" s="12">
         <f>_xll.qlRateHelperLatestDate($A13,Trigger)</f>
-        <v>42688</v>
+        <v>42731</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="str">
         <f>Swaps!L9</f>
-        <v>obj_00163#0003</v>
+        <v>obj_0012c#0001</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A14)</f>
@@ -2685,17 +2685,17 @@
       </c>
       <c r="H14" s="11">
         <f>_xll.qlRateHelperEarliestDate($A14,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I14" s="12">
         <f>_xll.qlRateHelperLatestDate($A14,Trigger)</f>
-        <v>42779</v>
+        <v>42821</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="str">
         <f>Swaps!L10</f>
-        <v>obj_00160#0003</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A15)</f>
@@ -2721,17 +2721,17 @@
       </c>
       <c r="H15" s="11">
         <f>_xll.qlRateHelperEarliestDate($A15,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I15" s="12">
         <f>_xll.qlRateHelperLatestDate($A15,Trigger)</f>
-        <v>42867</v>
+        <v>42912</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="str">
         <f>Swaps!L11</f>
-        <v>obj_0015d#0003</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A16)</f>
@@ -2757,17 +2757,17 @@
       </c>
       <c r="H16" s="11">
         <f>_xll.qlRateHelperEarliestDate($A16,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I16" s="12">
         <f>_xll.qlRateHelperLatestDate($A16,Trigger)</f>
-        <v>43234</v>
+        <v>43277</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="str">
         <f>Swaps!L12</f>
-        <v>obj_0015a#0003</v>
+        <v>obj_00131#0001</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A17)</f>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="C17" s="5">
         <f>_xll.qlRateHelperQuoteValue($A17,Trigger)</f>
-        <v>1.38E-2</v>
+        <v>1.3900000000000001E-2</v>
       </c>
       <c r="D17" s="5">
         <f>_xll.qlSwapRateHelperSpread($A17,Trigger)</f>
@@ -2793,17 +2793,17 @@
       </c>
       <c r="H17" s="11">
         <f>_xll.qlRateHelperEarliestDate($A17,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I17" s="12">
         <f>_xll.qlRateHelperLatestDate($A17,Trigger)</f>
-        <v>43598</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="str">
         <f>Swaps!L13</f>
-        <v>obj_0016c#0003</v>
+        <v>obj_00123#0001</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A18)</f>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="C18" s="5">
         <f>_xll.qlRateHelperQuoteValue($A18,Trigger)</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.6200000000000003E-2</v>
       </c>
       <c r="D18" s="5">
         <f>_xll.qlSwapRateHelperSpread($A18,Trigger)</f>
@@ -2829,17 +2829,17 @@
       </c>
       <c r="H18" s="11">
         <f>_xll.qlRateHelperEarliestDate($A18,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I18" s="12">
         <f>_xll.qlRateHelperLatestDate($A18,Trigger)</f>
-        <v>43963</v>
+        <v>44008</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="str">
         <f>Swaps!L14</f>
-        <v>obj_0016a#0003</v>
+        <v>obj_00125#0001</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A19)</f>
@@ -2865,17 +2865,17 @@
       </c>
       <c r="H19" s="11">
         <f>_xll.qlRateHelperEarliestDate($A19,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I19" s="12">
         <f>_xll.qlRateHelperLatestDate($A19,Trigger)</f>
-        <v>44328</v>
+        <v>44375</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="str">
         <f>Swaps!L15</f>
-        <v>obj_00168#0003</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A20)</f>
@@ -2883,7 +2883,7 @@
       </c>
       <c r="C20" s="5">
         <f>_xll.qlRateHelperQuoteValue($A20,Trigger)</f>
-        <v>1.8200000000000001E-2</v>
+        <v>1.9300000000000001E-2</v>
       </c>
       <c r="D20" s="5">
         <f>_xll.qlSwapRateHelperSpread($A20,Trigger)</f>
@@ -2901,17 +2901,17 @@
       </c>
       <c r="H20" s="11">
         <f>_xll.qlRateHelperEarliestDate($A20,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I20" s="12">
         <f>_xll.qlRateHelperLatestDate($A20,Trigger)</f>
-        <v>44693</v>
+        <v>44739</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="str">
         <f>Swaps!L16</f>
-        <v>obj_00165#0003</v>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A21)</f>
@@ -2937,17 +2937,17 @@
       </c>
       <c r="H21" s="11">
         <f>_xll.qlRateHelperEarliestDate($A21,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I21" s="12">
         <f>_xll.qlRateHelperLatestDate($A21,Trigger)</f>
-        <v>45058</v>
+        <v>45103</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="str">
         <f>Swaps!L17</f>
-        <v>obj_00162#0003</v>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A22)</f>
@@ -2973,17 +2973,17 @@
       </c>
       <c r="H22" s="11">
         <f>_xll.qlRateHelperEarliestDate($A22,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I22" s="12">
         <f>_xll.qlRateHelperLatestDate($A22,Trigger)</f>
-        <v>45425</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="str">
         <f>Swaps!L18</f>
-        <v>obj_0015f#0003</v>
+        <v>obj_00122#0001</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A23)</f>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="C23" s="5">
         <f>_xll.qlRateHelperQuoteValue($A23,Trigger)</f>
-        <v>2.06E-2</v>
+        <v>2.2099999999999998E-2</v>
       </c>
       <c r="D23" s="5">
         <f>_xll.qlSwapRateHelperSpread($A23,Trigger)</f>
@@ -3009,17 +3009,17 @@
       </c>
       <c r="H23" s="11">
         <f>_xll.qlRateHelperEarliestDate($A23,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I23" s="12">
         <f>_xll.qlRateHelperLatestDate($A23,Trigger)</f>
-        <v>45789</v>
+        <v>45834</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="str">
         <f>Swaps!L19</f>
-        <v>obj_0015c#0003</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A24)</f>
@@ -3045,17 +3045,17 @@
       </c>
       <c r="H24" s="11">
         <f>_xll.qlRateHelperEarliestDate($A24,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I24" s="12">
         <f>_xll.qlRateHelperLatestDate($A24,Trigger)</f>
-        <v>46154</v>
+        <v>46199</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="str">
         <f>Swaps!L20</f>
-        <v>obj_00159#0003</v>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A25)</f>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="C25" s="5">
         <f>_xll.qlRateHelperQuoteValue($A25,Trigger)</f>
-        <v>2.1399999999999995E-2</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="D25" s="5">
         <f>_xll.qlSwapRateHelperSpread($A25,Trigger)</f>
@@ -3081,17 +3081,17 @@
       </c>
       <c r="H25" s="11">
         <f>_xll.qlRateHelperEarliestDate($A25,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I25" s="12">
         <f>_xll.qlRateHelperLatestDate($A25,Trigger)</f>
-        <v>46519</v>
+        <v>46566</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="str">
         <f>Swaps!L21</f>
-        <v>obj_0016b#0003</v>
+        <v>obj_00124#0001</v>
       </c>
       <c r="B26" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A26)</f>
@@ -3117,17 +3117,17 @@
       </c>
       <c r="H26" s="11">
         <f>_xll.qlRateHelperEarliestDate($A26,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I26" s="12">
         <f>_xll.qlRateHelperLatestDate($A26,Trigger)</f>
-        <v>46885</v>
+        <v>46930</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="str">
         <f>Swaps!L22</f>
-        <v>obj_0016d#0003</v>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="B27" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A27)</f>
@@ -3153,17 +3153,17 @@
       </c>
       <c r="H27" s="11">
         <f>_xll.qlRateHelperEarliestDate($A27,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I27" s="12">
         <f>_xll.qlRateHelperLatestDate($A27,Trigger)</f>
-        <v>47252</v>
+        <v>47295</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="str">
         <f>Swaps!L23</f>
-        <v>obj_00167#0003</v>
+        <v>obj_00121#0001</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A28)</f>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="C28" s="5">
         <f>_xll.qlRateHelperQuoteValue($A28,Trigger)</f>
-        <v>2.2199999999999998E-2</v>
+        <v>2.3700000000000002E-2</v>
       </c>
       <c r="D28" s="5">
         <f>_xll.qlSwapRateHelperSpread($A28,Trigger)</f>
@@ -3189,17 +3189,17 @@
       </c>
       <c r="H28" s="11">
         <f>_xll.qlRateHelperEarliestDate($A28,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I28" s="12">
         <f>_xll.qlRateHelperLatestDate($A28,Trigger)</f>
-        <v>47616</v>
+        <v>47660</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="str">
         <f>Swaps!L24</f>
-        <v>obj_00164#0003</v>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A29)</f>
@@ -3225,17 +3225,17 @@
       </c>
       <c r="H29" s="11">
         <f>_xll.qlRateHelperEarliestDate($A29,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I29" s="12">
         <f>_xll.qlRateHelperLatestDate($A29,Trigger)</f>
-        <v>47980</v>
+        <v>48025</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="str">
         <f>Swaps!L25</f>
-        <v>obj_00161#0003</v>
+        <v>obj_00126#0001</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A30)</f>
@@ -3261,17 +3261,17 @@
       </c>
       <c r="H30" s="11">
         <f>_xll.qlRateHelperEarliestDate($A30,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I30" s="12">
         <f>_xll.qlRateHelperLatestDate($A30,Trigger)</f>
-        <v>48346</v>
+        <v>48393</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="str">
         <f>Swaps!L26</f>
-        <v>obj_0015e#0003</v>
+        <v>obj_00129#0001</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A31)</f>
@@ -3297,17 +3297,17 @@
       </c>
       <c r="H31" s="11">
         <f>_xll.qlRateHelperEarliestDate($A31,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I31" s="12">
         <f>_xll.qlRateHelperLatestDate($A31,Trigger)</f>
-        <v>48711</v>
+        <v>48757</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="str">
         <f>Swaps!L27</f>
-        <v>obj_0015b#0003</v>
+        <v>obj_00132#0001</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A32)</f>
@@ -3333,17 +3333,17 @@
       </c>
       <c r="H32" s="11">
         <f>_xll.qlRateHelperEarliestDate($A32,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I32" s="12">
         <f>_xll.qlRateHelperLatestDate($A32,Trigger)</f>
-        <v>49076</v>
+        <v>49121</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="str">
         <f>Swaps!L28</f>
-        <v>obj_00158#0003</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>_xll.qlRateHelperQuoteName(A33)</f>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="C33" s="5">
         <f>_xll.qlRateHelperQuoteValue($A33,Trigger)</f>
-        <v>2.35E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D33" s="5">
         <f>_xll.qlSwapRateHelperSpread($A33,Trigger)</f>
@@ -3369,11 +3369,11 @@
       </c>
       <c r="H33" s="11">
         <f>_xll.qlRateHelperEarliestDate($A33,Trigger)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I33" s="12">
         <f>_xll.qlRateHelperLatestDate($A33,Trigger)</f>
-        <v>49443</v>
+        <v>49486</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3454,15 +3454,15 @@
       </c>
       <c r="D2" s="21" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
-        <v>obj_00128</v>
+        <v>obj_00140</v>
       </c>
       <c r="E2" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D2)</f>
-        <v>HkdHibor6MLastFixing_Quote</v>
+        <v>HKD6MD_Quote</v>
       </c>
       <c r="F2" s="22">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>5.4136000000000011E-3</v>
+        <v>5.4286000000000004E-3</v>
       </c>
       <c r="G2" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -3470,14 +3470,14 @@
       </c>
       <c r="H2" s="11">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="I2" s="28">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>42319</v>
+        <v>42366</v>
       </c>
       <c r="J2" s="18">
-        <v>0.99727837976014466</v>
+        <v>0.9972412765401325</v>
       </c>
       <c r="K2" s="23"/>
     </row>
@@ -3489,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="21" t="str">
-        <v>obj_00157</v>
+        <v>obj_00127</v>
       </c>
       <c r="E3" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D3)</f>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="F3" s="22">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>5.3E-3</v>
       </c>
       <c r="G3" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -3505,14 +3505,14 @@
       </c>
       <c r="H3" s="11">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I3" s="28">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>42502</v>
+        <v>42548</v>
       </c>
       <c r="J3" s="18">
-        <v>0.99518544388735097</v>
+        <v>0.99467307832788687</v>
       </c>
       <c r="K3" s="23"/>
     </row>
@@ -3524,7 +3524,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="21" t="str">
-        <v>obj_00166</v>
+        <v>obj_00128</v>
       </c>
       <c r="E4" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D4)</f>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="F4" s="22">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>6.5000000000000006E-3</v>
+        <v>6.6999999999999994E-3</v>
       </c>
       <c r="G4" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -3540,14 +3540,14 @@
       </c>
       <c r="H4" s="11">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I4" s="28">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>42688</v>
+        <v>42731</v>
       </c>
       <c r="J4" s="18">
-        <v>0.99020156077964427</v>
+        <v>0.9899402846901465</v>
       </c>
       <c r="K4" s="23"/>
     </row>
@@ -3559,7 +3559,7 @@
         <v>63</v>
       </c>
       <c r="D5" s="21" t="str">
-        <v>obj_00160</v>
+        <v>obj_00136</v>
       </c>
       <c r="E5" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D5)</f>
@@ -3575,14 +3575,14 @@
       </c>
       <c r="H5" s="11">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I5" s="28">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>42867</v>
+        <v>42912</v>
       </c>
       <c r="J5" s="18">
-        <v>0.98348239095329704</v>
+        <v>0.98348675808599173</v>
       </c>
       <c r="K5" s="23"/>
     </row>
@@ -3590,7 +3590,7 @@
       <c r="A6" s="54"/>
       <c r="B6" s="54"/>
       <c r="D6" s="21" t="str">
-        <v>obj_0015d</v>
+        <v>obj_00134</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D6)</f>
@@ -3606,20 +3606,20 @@
       </c>
       <c r="H6" s="11">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I6" s="28">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>43234</v>
+        <v>43277</v>
       </c>
       <c r="J6" s="18">
-        <v>0.9661666072078946</v>
+        <v>0.96623222939470677</v>
       </c>
       <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="21" t="str">
-        <v>obj_0015a</v>
+        <v>obj_00131</v>
       </c>
       <c r="E7" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D7)</f>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="F7" s="22">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.38E-2</v>
+        <v>1.3900000000000001E-2</v>
       </c>
       <c r="G7" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -3635,20 +3635,20 @@
       </c>
       <c r="H7" s="11">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I7" s="28">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>43598</v>
+        <v>43642</v>
       </c>
       <c r="J7" s="18">
-        <v>0.94592267064079705</v>
+        <v>0.94557552754721896</v>
       </c>
       <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="str">
-        <v>obj_0016c</v>
+        <v>obj_00123</v>
       </c>
       <c r="E8" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D8)</f>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="F8" s="22">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.6200000000000003E-2</v>
       </c>
       <c r="G8" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -3664,20 +3664,20 @@
       </c>
       <c r="H8" s="11">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I8" s="28">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>43963</v>
+        <v>44008</v>
       </c>
       <c r="J8" s="18">
-        <v>0.92432436413541419</v>
+        <v>0.92145460157204218</v>
       </c>
       <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="21" t="str">
-        <v>obj_00168</v>
+        <v>obj_00137</v>
       </c>
       <c r="E9" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D9)</f>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="F9" s="22">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1.8200000000000001E-2</v>
+        <v>1.9300000000000001E-2</v>
       </c>
       <c r="G9" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -3693,20 +3693,20 @@
       </c>
       <c r="H9" s="11">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I9" s="28">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="J9" s="18">
-        <v>0.87899113195046319</v>
+        <v>0.87188440298917702</v>
       </c>
       <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="21" t="str">
-        <v>obj_0015f</v>
+        <v>obj_00122</v>
       </c>
       <c r="E10" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D10)</f>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="F10" s="22">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>2.06E-2</v>
+        <v>2.2099999999999998E-2</v>
       </c>
       <c r="G10" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -3722,20 +3722,20 @@
       </c>
       <c r="H10" s="11">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I10" s="28">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>45789</v>
+        <v>45834</v>
       </c>
       <c r="J10" s="18">
-        <v>0.81096864568402427</v>
+        <v>0.79819693203697051</v>
       </c>
       <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="21" t="str">
-        <v>obj_00159</v>
+        <v>obj_0012e</v>
       </c>
       <c r="E11" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D11)</f>
@@ -3743,7 +3743,7 @@
       </c>
       <c r="F11" s="22">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>2.1399999999999995E-2</v>
+        <v>2.2700000000000001E-2</v>
       </c>
       <c r="G11" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -3751,20 +3751,20 @@
       </c>
       <c r="H11" s="11">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I11" s="28">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>46519</v>
+        <v>46566</v>
       </c>
       <c r="J11" s="18">
-        <v>0.76991953253976941</v>
+        <v>0.75743861606421581</v>
       </c>
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="str">
-        <v>obj_00167</v>
+        <v>obj_00121</v>
       </c>
       <c r="E12" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D12)</f>
@@ -3772,7 +3772,7 @@
       </c>
       <c r="F12" s="22">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>2.2199999999999998E-2</v>
+        <v>2.3700000000000002E-2</v>
       </c>
       <c r="G12" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -3780,20 +3780,20 @@
       </c>
       <c r="H12" s="11">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I12" s="28">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>47616</v>
+        <v>47660</v>
       </c>
       <c r="J12" s="18">
-        <v>0.71204963895355788</v>
+        <v>0.69532824631967038</v>
       </c>
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="21" t="str">
-        <v>obj_00158</v>
+        <v>obj_00135</v>
       </c>
       <c r="E13" s="21" t="str">
         <f>_xll.qlRateHelperQuoteName(D13)</f>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="F13" s="22">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>2.35E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G13" s="22">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),0,_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -3809,14 +3809,14 @@
       </c>
       <c r="H13" s="11">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>42136</v>
+        <v>42181</v>
       </c>
       <c r="I13" s="28">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>49443</v>
+        <v>49486</v>
       </c>
       <c r="J13" s="18">
-        <v>0.61733372763186234</v>
+        <v>0.59816766612848471</v>
       </c>
       <c r="K13" s="23"/>
     </row>
@@ -7007,7 +7007,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7015,8 +7015,8 @@
     <col min="1" max="1" width="2.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="35.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
@@ -7068,12 +7068,12 @@
         <v>HkdHiborON</v>
       </c>
       <c r="D3" s="38" t="str">
-        <f t="shared" ref="D3:D11" si="1">PROPER(Currency)&amp;FamilyName&amp;$B3&amp;"LastFixing"&amp;QuoteSuffix</f>
-        <v>HkdHiborONLastFixing_Quote</v>
+        <f>Currency&amp;$B3&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKDOND_Quote</v>
       </c>
       <c r="E3" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00121#0002</v>
+        <v>obj_00138#0005</v>
       </c>
       <c r="F3" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E3)</f>
@@ -7093,12 +7093,12 @@
         <v>HkdHiborSW</v>
       </c>
       <c r="D4" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHiborSWLastFixing_Quote</v>
+        <f>Currency&amp;$B4&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKDSWD_Quote</v>
       </c>
       <c r="E4" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00127#0002</v>
+        <v>obj_0013f#0003</v>
       </c>
       <c r="F4" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E4)</f>
@@ -7118,12 +7118,12 @@
         <v>HkdHibor2W</v>
       </c>
       <c r="D5" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor2WLastFixing_Quote</v>
+        <f>Currency&amp;$B5&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD2WD_Quote</v>
       </c>
       <c r="E5" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00126#0002</v>
+        <v>obj_0013e#0003</v>
       </c>
       <c r="F5" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E5)</f>
@@ -7143,12 +7143,12 @@
         <v>HkdHibor1M</v>
       </c>
       <c r="D6" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor1MLastFixing_Quote</v>
+        <f>Currency&amp;$B6&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD1MD_Quote</v>
       </c>
       <c r="E6" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00129#0002</v>
+        <v>obj_00139#0003</v>
       </c>
       <c r="F6" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E6)</f>
@@ -7168,12 +7168,12 @@
         <v>HkdHibor2M</v>
       </c>
       <c r="D7" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor2MLastFixing_Quote</v>
+        <f>Currency&amp;$B7&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD2MD_Quote</v>
       </c>
       <c r="E7" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00125#0002</v>
+        <v>obj_0013d#0003</v>
       </c>
       <c r="F7" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E7)</f>
@@ -7193,12 +7193,12 @@
         <v>HkdHibor3M</v>
       </c>
       <c r="D8" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor3MLastFixing_Quote</v>
+        <f>Currency&amp;$B8&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD3MD_Quote</v>
       </c>
       <c r="E8" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00122#0002</v>
+        <v>obj_0013a#0003</v>
       </c>
       <c r="F8" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E8)</f>
@@ -7218,12 +7218,12 @@
         <v>HkdHibor6M</v>
       </c>
       <c r="D9" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor6MLastFixing_Quote</v>
+        <f>Currency&amp;$B9&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD6MD_Quote</v>
       </c>
       <c r="E9" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00128#0002</v>
+        <v>obj_00140#0003</v>
       </c>
       <c r="F9" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E9)</f>
@@ -7243,12 +7243,12 @@
         <v>HkdHibor9M</v>
       </c>
       <c r="D10" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor9MLastFixing_Quote</v>
+        <f>Currency&amp;$B10&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD9MD_Quote</v>
       </c>
       <c r="E10" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00124#0002</v>
+        <v>obj_0013c#0003</v>
       </c>
       <c r="F10" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E10)</f>
@@ -7268,12 +7268,12 @@
         <v>HkdHibor1Y</v>
       </c>
       <c r="D11" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>HkdHibor1YLastFixing_Quote</v>
+        <f>Currency&amp;$B11&amp;"D"&amp;QuoteSuffix</f>
+        <v>HKD1YD_Quote</v>
       </c>
       <c r="E11" s="37" t="str">
         <f>_xll.qlDepositRateHelper(,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00123#0002</v>
+        <v>obj_0013b#0003</v>
       </c>
       <c r="F11" s="36" t="str">
         <f>_xll.ohRangeRetrieveError(E11)</f>
@@ -7441,7 +7441,7 @@
       <c r="K4" s="48"/>
       <c r="L4" s="63" t="str">
         <f>_xll.qlIborIndex(,FamilyName,J2,P4,Currency,Q4,R4,S4,T4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00120#0003</v>
+        <v>obj_00120#0001</v>
       </c>
       <c r="M4" s="64" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -7520,7 +7520,7 @@
       </c>
       <c r="L6" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K6,$B6,$D6,Calendar,$G6,$H6,$I6,$L$4,$J6,C6&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00157#0003</v>
+        <v>obj_00127#0001</v>
       </c>
       <c r="M6" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="L7" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K7,$B7,$D7,Calendar,$G7,$H7,$I7,$L$4,$J7,C7&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00169#0003</v>
+        <v>obj_00130#0001</v>
       </c>
       <c r="M7" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="L8" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K8,$B8,$D8,Calendar,$G8,$H8,$I8,$L$4,$J8,C8&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00166#0003</v>
+        <v>obj_00128#0001</v>
       </c>
       <c r="M8" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -7658,7 +7658,7 @@
       </c>
       <c r="L9" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K9,$B9,$D9,Calendar,$G9,$H9,$I9,$L$4,$J9,C9&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00163#0003</v>
+        <v>obj_0012c#0001</v>
       </c>
       <c r="M9" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -7704,7 +7704,7 @@
       </c>
       <c r="L10" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K10,$B10,$D10,Calendar,$G10,$H10,$I10,$L$4,$J10,C10&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00160#0003</v>
+        <v>obj_00136#0001</v>
       </c>
       <c r="M10" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="L11" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K11,$B11,$D11,Calendar,$G11,$H11,$I11,$L$4,$J11,C11&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015d#0003</v>
+        <v>obj_00134#0001</v>
       </c>
       <c r="M11" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -7796,7 +7796,7 @@
       </c>
       <c r="L12" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K12,$B12,$D12,Calendar,$G12,$H12,$I12,$L$4,$J12,C12&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015a#0003</v>
+        <v>obj_00131#0001</v>
       </c>
       <c r="M12" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -7842,7 +7842,7 @@
       </c>
       <c r="L13" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K13,$B13,$D13,Calendar,$G13,$H13,$I13,$L$4,$J13,C13&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0016c#0003</v>
+        <v>obj_00123#0001</v>
       </c>
       <c r="M13" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -7888,7 +7888,7 @@
       </c>
       <c r="L14" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K14,$B14,$D14,Calendar,$G14,$H14,$I14,$L$4,$J14,C14&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0016a#0003</v>
+        <v>obj_00125#0001</v>
       </c>
       <c r="M14" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="L15" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K15,$B15,$D15,Calendar,$G15,$H15,$I15,$L$4,$J15,C15&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00168#0003</v>
+        <v>obj_00137#0001</v>
       </c>
       <c r="M15" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -7980,7 +7980,7 @@
       </c>
       <c r="L16" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K16,$B16,$D16,Calendar,$G16,$H16,$I16,$L$4,$J16,C16&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00165#0003</v>
+        <v>obj_0012a#0001</v>
       </c>
       <c r="M16" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -8026,7 +8026,7 @@
       </c>
       <c r="L17" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K17,$B17,$D17,Calendar,$G17,$H17,$I17,$L$4,$J17,C17&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00162#0003</v>
+        <v>obj_0012d#0001</v>
       </c>
       <c r="M17" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -8072,7 +8072,7 @@
       </c>
       <c r="L18" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K18,$B18,$D18,Calendar,$G18,$H18,$I18,$L$4,$J18,C18&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015f#0003</v>
+        <v>obj_00122#0001</v>
       </c>
       <c r="M18" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -8118,7 +8118,7 @@
       </c>
       <c r="L19" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K19,$B19,$D19,Calendar,$G19,$H19,$I19,$L$4,$J19,C19&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015c#0003</v>
+        <v>obj_00133#0001</v>
       </c>
       <c r="M19" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -8164,7 +8164,7 @@
       </c>
       <c r="L20" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K20,$B20,$D20,Calendar,$G20,$H20,$I20,$L$4,$J20,C20&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00159#0003</v>
+        <v>obj_0012e#0001</v>
       </c>
       <c r="M20" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -8210,7 +8210,7 @@
       </c>
       <c r="L21" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K21,$B21,$D21,Calendar,$G21,$H21,$I21,$L$4,$J21,C21&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0016b#0003</v>
+        <v>obj_00124#0001</v>
       </c>
       <c r="M21" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -8256,7 +8256,7 @@
       </c>
       <c r="L22" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K22,$B22,$D22,Calendar,$G22,$H22,$I22,$L$4,$J22,C22&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0016d#0003</v>
+        <v>obj_0012f#0001</v>
       </c>
       <c r="M22" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -8302,7 +8302,7 @@
       </c>
       <c r="L23" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K23,$B23,$D23,Calendar,$G23,$H23,$I23,$L$4,$J23,C23&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00167#0003</v>
+        <v>obj_00121#0001</v>
       </c>
       <c r="M23" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -8348,7 +8348,7 @@
       </c>
       <c r="L24" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K24,$B24,$D24,Calendar,$G24,$H24,$I24,$L$4,$J24,C24&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00164#0003</v>
+        <v>obj_0012b#0001</v>
       </c>
       <c r="M24" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -8394,7 +8394,7 @@
       </c>
       <c r="L25" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K25,$B25,$D25,Calendar,$G25,$H25,$I25,$L$4,$J25,C25&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00161#0003</v>
+        <v>obj_00126#0001</v>
       </c>
       <c r="M25" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -8440,7 +8440,7 @@
       </c>
       <c r="L26" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K26,$B26,$D26,Calendar,$G26,$H26,$I26,$L$4,$J26,C26&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015e#0003</v>
+        <v>obj_00129#0001</v>
       </c>
       <c r="M26" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -8486,7 +8486,7 @@
       </c>
       <c r="L27" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K27,$B27,$D27,Calendar,$G27,$H27,$I27,$L$4,$J27,C27&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_0015b#0003</v>
+        <v>obj_00132#0001</v>
       </c>
       <c r="M27" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -8532,7 +8532,7 @@
       </c>
       <c r="L28" s="71" t="str">
         <f>_xll.qlSwapRateHelper2(,$K28,$B28,$D28,Calendar,$G28,$H28,$I28,$L$4,$J28,C28&amp;"D",Discounting2,Permanent,,ObjectOverwrite)</f>
-        <v>obj_00158#0003</v>
+        <v>obj_00135#0001</v>
       </c>
       <c r="M28" s="61" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>

</xml_diff>